<commit_message>
added manual feature classifications to excel tables
</commit_message>
<xml_diff>
--- a/scripts/deduplicate_project/results/excel/axtls_2_1_4_infer.xlsx
+++ b/scripts/deduplicate_project/results/excel/axtls_2_1_4_infer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hothost/Documents/git/kconfig_case_studies/scripts/deduplicate_project/results/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austin/Documents/kconfig_case_studies/scripts/deduplicate_project/results/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D628A4DA-A809-1F4C-8713-AB908F7C9AA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA9C045-7E6F-674B-8A0E-15A7E24EB20C}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="13860" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,13 +18,15 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="41">
   <si>
     <t>line</t>
   </si>
@@ -125,13 +127,43 @@
   </si>
   <si>
     <t>Count of variability2</t>
+  </si>
+  <si>
+    <t>manual_features</t>
+  </si>
+  <si>
+    <t>num_manual_features</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>AXHTTPD</t>
+  </si>
+  <si>
+    <t>BIGINT_SLIDING_WINDOW</t>
+  </si>
+  <si>
+    <t>AXHTTPD,HTTP_HAS_CGI,(!CONFIG_PLATFORM_WIN32)</t>
+  </si>
+  <si>
+    <t>AXHTTPD, HTTP_HAS_AUTHORIZATION,(-CONFIG_C_SAMPLES)</t>
+  </si>
+  <si>
+    <t>OPENSSL_COMPATIBLE</t>
+  </si>
+  <si>
+    <t>SSL_HAS_PEM</t>
+  </si>
+  <si>
+    <t>SSL_USE_PKCS12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -608,7 +640,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -616,6 +648,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1182,7 +1215,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable6" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1242,12 +1275,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H48" totalsRowCount="1">
-  <autoFilter ref="A1:H47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
-    <sortCondition descending="1" ref="F1:F47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J48" totalsRowCount="1">
+  <autoFilter ref="A1:J47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J47">
+    <sortCondition ref="B1:B47"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="line"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="filename"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="tool"/>
@@ -1258,6 +1291,8 @@
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="variability"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="classification"/>
+    <tableColumn id="9" xr3:uid="{F78777BA-15C0-A145-99F2-E84FD23826E1}" name="manual_features"/>
+    <tableColumn id="10" xr3:uid="{0278CB9B-A8B5-1846-A987-BE62C0F7F88C}" name="num_manual_features"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1566,14 +1601,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1584,7 +1619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1595,7 +1630,7 @@
         <v>0.56521739130434778</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1606,7 +1641,7 @@
         <v>0.43478260869565216</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1624,20 +1659,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1662,8 +1697,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>276</v>
       </c>
@@ -1689,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>286</v>
       </c>
@@ -1715,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>301</v>
       </c>
@@ -1741,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>315</v>
       </c>
@@ -1767,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>326</v>
       </c>
@@ -1793,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>335</v>
       </c>
@@ -1819,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>344</v>
       </c>
@@ -1845,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>104</v>
       </c>
@@ -1870,8 +1911,11 @@
       <c r="H9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>105</v>
       </c>
@@ -1896,8 +1940,11 @@
       <c r="H10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>252</v>
       </c>
@@ -1922,8 +1969,11 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>265</v>
       </c>
@@ -1948,8 +1998,11 @@
       <c r="H12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>627</v>
       </c>
@@ -1974,8 +2027,11 @@
       <c r="H13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>826</v>
       </c>
@@ -2000,8 +2056,11 @@
       <c r="H14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>1112</v>
       </c>
@@ -2026,13 +2085,16 @@
       <c r="H15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
-        <v>489</v>
+        <v>1319</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -2044,21 +2106,27 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <v>1000</v>
+        <v>497</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
-        <v>614</v>
+        <v>1373</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -2070,21 +2138,27 @@
         <v>13</v>
       </c>
       <c r="F17">
-        <v>1000</v>
+        <v>503</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
-        <v>169</v>
+        <v>295</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -2093,24 +2167,21 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F18">
-        <v>1000</v>
+        <v>98</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
-        <v>457</v>
+        <v>476</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -2122,21 +2193,27 @@
         <v>13</v>
       </c>
       <c r="F19">
-        <v>1000</v>
+        <v>527</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
-        <v>459</v>
+        <v>479</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -2148,21 +2225,27 @@
         <v>13</v>
       </c>
       <c r="F20">
-        <v>1000</v>
+        <v>527</v>
       </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
-        <v>464</v>
+        <v>489</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -2182,13 +2265,19 @@
       <c r="H21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
-        <v>72</v>
+        <v>614</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -2208,13 +2297,19 @@
       <c r="H22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -2226,21 +2321,27 @@
         <v>13</v>
       </c>
       <c r="F23">
-        <v>1000</v>
+        <v>307</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -2249,24 +2350,30 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F24">
-        <v>1000</v>
+        <v>307</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
-        <v>169</v>
+        <v>633</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -2275,24 +2382,24 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F25">
-        <v>1000</v>
+        <v>527</v>
       </c>
       <c r="G25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
-        <v>609</v>
+        <v>640</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -2301,24 +2408,24 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F26">
-        <v>1000</v>
+        <v>527</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
-        <v>1253</v>
+        <v>641</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -2327,21 +2434,24 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F27">
-        <v>1000</v>
+        <v>527</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
-        <v>476</v>
+        <v>669</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -2350,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F28">
         <v>527</v>
@@ -2359,15 +2469,15 @@
         <v>1</v>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
-        <v>479</v>
+        <v>670</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -2376,7 +2486,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F29">
         <v>527</v>
@@ -2385,12 +2495,12 @@
         <v>1</v>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
-        <v>633</v>
+        <v>671</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -2414,12 +2524,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31">
-        <v>640</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -2428,24 +2538,21 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F31">
-        <v>527</v>
+        <v>337</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
       </c>
-      <c r="H31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
-        <v>641</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -2454,24 +2561,27 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F32">
-        <v>527</v>
+        <v>1000</v>
       </c>
       <c r="G32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
-        <v>669</v>
+        <v>457</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -2480,24 +2590,27 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F33">
-        <v>527</v>
+        <v>1000</v>
       </c>
       <c r="G33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
-        <v>670</v>
+        <v>459</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -2506,24 +2619,27 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F34">
-        <v>527</v>
+        <v>1000</v>
       </c>
       <c r="G34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
-        <v>671</v>
+        <v>464</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -2532,24 +2648,27 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F35">
-        <v>527</v>
+        <v>1000</v>
       </c>
       <c r="G35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
-        <v>1373</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -2561,21 +2680,24 @@
         <v>13</v>
       </c>
       <c r="F36">
-        <v>503</v>
+        <v>1000</v>
       </c>
       <c r="G36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -2587,21 +2709,24 @@
         <v>13</v>
       </c>
       <c r="F37">
-        <v>501</v>
+        <v>1000</v>
       </c>
       <c r="G37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
-        <v>177</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -2613,21 +2738,24 @@
         <v>13</v>
       </c>
       <c r="F38">
-        <v>501</v>
+        <v>1000</v>
       </c>
       <c r="G38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -2636,24 +2764,24 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F39">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
-        <v>1319</v>
+        <v>406</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -2665,7 +2793,7 @@
         <v>13</v>
       </c>
       <c r="F40">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -2673,8 +2801,14 @@
       <c r="H40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>69</v>
       </c>
@@ -2699,13 +2833,19 @@
       <c r="H41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
-        <v>330</v>
+        <v>173</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -2714,24 +2854,30 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F42">
-        <v>482</v>
+        <v>501</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
       </c>
       <c r="H42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>40</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
-        <v>406</v>
+        <v>177</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -2743,7 +2889,7 @@
         <v>13</v>
       </c>
       <c r="F43">
-        <v>482</v>
+        <v>501</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
@@ -2751,13 +2897,19 @@
       <c r="H43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>40</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
-        <v>151</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -2769,18 +2921,27 @@
         <v>13</v>
       </c>
       <c r="F44">
-        <v>337</v>
+        <v>501</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -2792,21 +2953,24 @@
         <v>13</v>
       </c>
       <c r="F45">
-        <v>307</v>
+        <v>1000</v>
       </c>
       <c r="G45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
-        <v>135</v>
+        <v>609</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -2815,24 +2979,27 @@
         <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F46">
-        <v>307</v>
+        <v>1000</v>
       </c>
       <c r="G46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
-        <v>295</v>
+        <v>1253</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -2844,16 +3011,16 @@
         <v>15</v>
       </c>
       <c r="F47">
-        <v>98</v>
+        <v>1000</v>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="F48">
         <f>MEDIAN(F28:F47)</f>
-        <v>501</v>
+        <v>763.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>